<commit_message>
Fix test excel files
</commit_message>
<xml_diff>
--- a/tests/data/checker/example07_codeexists_objtype_warningdefschanged.xlsx
+++ b/tests/data/checker/example07_codeexists_objtype_warningdefschanged.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\0Work\07_BAM\work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpizarro\work\repos\bam-masterdata\tests\data\checker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A108E77-6400-4012-8888-518DDE0CA782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D804FD5-B2C1-411F-A01D-92BE6EBEB244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object types" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>ACTION</t>
   </si>
   <si>
-    <t>Auto generated codes</t>
-  </si>
-  <si>
     <t>ACT</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Changed description (minor warning)</t>
+  </si>
+  <si>
+    <t>Auto generate codes</t>
   </si>
 </sst>
 </file>
@@ -487,10 +487,10 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -531,7 +531,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="G2"/>
       <c r="H2"/>
@@ -550,10 +550,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -576,7 +576,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>13</v>
@@ -594,10 +594,10 @@
         <v>9</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="O4"/>
       <c r="P4"/>
@@ -605,40 +605,40 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
         <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
       <c r="I6" t="s">
         <v>17</v>
       </c>
@@ -646,21 +646,21 @@
         <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
@@ -689,30 +689,30 @@
         <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>